<commit_message>
Update charts for July 18th
</commit_message>
<xml_diff>
--- a/Data/MDCOVID19_CasesByAgeDistribution.xlsx
+++ b/Data/MDCOVID19_CasesByAgeDistribution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb61959dcc1c374c/Documents/GitHub/MD-COVID19/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{8C2F2433-59D0-42E7-B955-80569FABD71F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5A3CEEA6-378A-4357-8581-051828FB6CF2}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{8C2F2433-59D0-42E7-B955-80569FABD71F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{483C0409-BEE7-4799-946F-E8694315F4B6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -916,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="C115" sqref="C115"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12507,7 +12507,114 @@
         <v>14.428571428571429</v>
       </c>
     </row>
-    <row r="114" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>111</v>
+      </c>
+      <c r="B113" s="2">
+        <v>44029</v>
+      </c>
+      <c r="C113">
+        <v>2427</v>
+      </c>
+      <c r="D113">
+        <v>4267</v>
+      </c>
+      <c r="E113">
+        <v>12178</v>
+      </c>
+      <c r="F113">
+        <v>14309</v>
+      </c>
+      <c r="G113">
+        <v>13248</v>
+      </c>
+      <c r="H113">
+        <v>11727</v>
+      </c>
+      <c r="I113">
+        <v>8286</v>
+      </c>
+      <c r="J113">
+        <v>5192</v>
+      </c>
+      <c r="K113">
+        <v>4737</v>
+      </c>
+      <c r="M113">
+        <f t="shared" ref="M113" si="56">SUM(C113-C112)</f>
+        <v>40</v>
+      </c>
+      <c r="N113">
+        <f t="shared" ref="N113" si="57">SUM(D113-D112)</f>
+        <v>60</v>
+      </c>
+      <c r="O113">
+        <f t="shared" ref="O113" si="58">SUM(E113-E112)</f>
+        <v>206</v>
+      </c>
+      <c r="P113">
+        <f t="shared" ref="P113" si="59">SUM(F113-F112)</f>
+        <v>126</v>
+      </c>
+      <c r="Q113">
+        <f t="shared" ref="Q113" si="60">SUM(G113-G112)</f>
+        <v>106</v>
+      </c>
+      <c r="R113">
+        <f t="shared" ref="R113" si="61">SUM(H113-H112)</f>
+        <v>88</v>
+      </c>
+      <c r="S113">
+        <f t="shared" ref="S113" si="62">SUM(I113-I112)</f>
+        <v>43</v>
+      </c>
+      <c r="T113">
+        <f t="shared" ref="T113" si="63">SUM(J113-J112)</f>
+        <v>19</v>
+      </c>
+      <c r="U113">
+        <f t="shared" ref="U113" si="64">SUM(K113-K112)</f>
+        <v>19</v>
+      </c>
+      <c r="W113" s="1">
+        <f t="shared" ref="W113" si="65">AVERAGE(M107:M113)</f>
+        <v>29</v>
+      </c>
+      <c r="X113" s="1">
+        <f t="shared" ref="X113" si="66">AVERAGE(N107:N113)</f>
+        <v>55.428571428571431</v>
+      </c>
+      <c r="Y113" s="1">
+        <f t="shared" ref="Y113" si="67">AVERAGE(O107:O113)</f>
+        <v>169</v>
+      </c>
+      <c r="Z113" s="1">
+        <f t="shared" ref="Z113" si="68">AVERAGE(P107:P113)</f>
+        <v>124</v>
+      </c>
+      <c r="AA113" s="1">
+        <f t="shared" ref="AA113" si="69">AVERAGE(Q107:Q113)</f>
+        <v>89.571428571428569</v>
+      </c>
+      <c r="AB113" s="1">
+        <f t="shared" ref="AB113" si="70">AVERAGE(R107:R113)</f>
+        <v>78.571428571428569</v>
+      </c>
+      <c r="AC113" s="1">
+        <f t="shared" ref="AC113" si="71">AVERAGE(S107:S113)</f>
+        <v>48.285714285714285</v>
+      </c>
+      <c r="AD113" s="1">
+        <f t="shared" ref="AD113" si="72">AVERAGE(T107:T113)</f>
+        <v>26.714285714285715</v>
+      </c>
+      <c r="AE113" s="1">
+        <f t="shared" ref="AE113" si="73">AVERAGE(U107:U113)</f>
+        <v>16.714285714285715</v>
+      </c>
+    </row>
+    <row r="114" spans="1:31" x14ac:dyDescent="0.25">
       <c r="V114" s="1"/>
       <c r="W114" s="1"/>
       <c r="X114" s="1"/>
@@ -12519,46 +12626,60 @@
       <c r="AD114" s="1"/>
       <c r="AE114" s="1"/>
     </row>
-    <row r="115" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:31" x14ac:dyDescent="0.25">
       <c r="V115" s="1"/>
       <c r="W115" s="1"/>
     </row>
-    <row r="116" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:31" x14ac:dyDescent="0.25">
       <c r="V116" s="1"/>
       <c r="W116" s="1"/>
     </row>
-    <row r="117" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:31" x14ac:dyDescent="0.25">
       <c r="V117" s="1"/>
       <c r="W117" s="1"/>
     </row>
-    <row r="118" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:31" x14ac:dyDescent="0.25">
       <c r="V118" s="1"/>
       <c r="W118" s="1"/>
     </row>
-    <row r="119" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:31" x14ac:dyDescent="0.25">
       <c r="V119" s="1"/>
       <c r="W119" s="1"/>
     </row>
-    <row r="120" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:31" x14ac:dyDescent="0.25">
       <c r="V120" s="1"/>
       <c r="W120" s="1"/>
     </row>
-    <row r="121" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:31" x14ac:dyDescent="0.25">
       <c r="V121" s="1"/>
       <c r="W121" s="1"/>
     </row>
-    <row r="122" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:31" x14ac:dyDescent="0.25">
       <c r="V122" s="1"/>
       <c r="W122" s="1"/>
     </row>
-    <row r="123" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:31" x14ac:dyDescent="0.25">
       <c r="V123" s="1"/>
-    </row>
-    <row r="128" spans="4:31" x14ac:dyDescent="0.25">
+      <c r="W123" s="1"/>
+    </row>
+    <row r="124" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W124" s="1"/>
+    </row>
+    <row r="125" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W125" s="1"/>
+    </row>
+    <row r="126" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W126" s="1"/>
+    </row>
+    <row r="127" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W127" s="1"/>
+    </row>
+    <row r="128" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
+      <c r="W128" s="1"/>
     </row>
     <row r="129" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D129" s="1"/>

</xml_diff>